<commit_message>
TICKET2383 * Updated Excel Spreadsheet
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3716 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-9.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-9.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4605" windowWidth="19440" windowHeight="5520" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="4605" windowWidth="19440" windowHeight="5520" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="4" state="hidden" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
   <si>
     <t>calls</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Each time a traveler contacts you directly, you have the opportunity to create a booking through your website or reservations desk.  Direct Bookings are approximated based on conservative conversion rates:  1 out of 100 clicks converts, 1 out of 25 calls converts.  Booking amount is average of an LLTG booking transaction for the time period.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">** See Key for Approximate Direct Bookings details.  </t>
   </si>
 </sst>
 </file>
@@ -1181,6 +1184,10 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="8" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1193,10 +1200,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="17" fontId="8" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1841,11 +1844,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="76542720"/>
-        <c:axId val="76544256"/>
+        <c:axId val="154645632"/>
+        <c:axId val="154647168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76542720"/>
+        <c:axId val="154645632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,7 +1876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76544256"/>
+        <c:crossAx val="154647168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1881,7 +1884,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76544256"/>
+        <c:axId val="154647168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1909,7 +1912,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="76542720"/>
+        <c:crossAx val="154645632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2208,12 +2211,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="79142912"/>
-        <c:axId val="79144448"/>
+        <c:axId val="73007488"/>
+        <c:axId val="73009024"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="79142912"/>
+        <c:axId val="73007488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,7 +2244,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79144448"/>
+        <c:crossAx val="73009024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2249,7 +2252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79144448"/>
+        <c:axId val="73009024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2277,7 +2280,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79142912"/>
+        <c:crossAx val="73007488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2495,12 +2498,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="80299520"/>
-        <c:axId val="80301056"/>
+        <c:axId val="73025408"/>
+        <c:axId val="73026944"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="80299520"/>
+        <c:axId val="73025408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2528,7 +2531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80301056"/>
+        <c:crossAx val="73026944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2536,7 +2539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80301056"/>
+        <c:axId val="73026944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2564,7 +2567,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80299520"/>
+        <c:crossAx val="73025408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2739,12 +2742,12 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="80331904"/>
-        <c:axId val="80333440"/>
+        <c:axId val="73043968"/>
+        <c:axId val="73045504"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="80331904"/>
+        <c:axId val="73043968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2764,7 +2767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80333440"/>
+        <c:crossAx val="73045504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2772,7 +2775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80333440"/>
+        <c:axId val="73045504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2782,7 +2785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80331904"/>
+        <c:crossAx val="73043968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4383,7 +4386,9 @@
   </sheetPr>
   <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6474,8 +6479,8 @@
   </sheetPr>
   <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6492,10 +6497,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="155" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="154"/>
+      <c r="B1" s="156"/>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -6530,7 +6535,7 @@
       <c r="I3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="154" t="s">
         <v>79</v>
       </c>
       <c r="B4" s="52" t="s">
@@ -6545,7 +6550,7 @@
       <c r="I4" s="37"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="161" t="s">
+      <c r="A5" s="154" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="52" t="s">
@@ -6819,20 +6824,38 @@
       <c r="A16" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="160">
+      <c r="B16" s="153">
         <f>(B12/25)+(B11/100)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="160">
+      <c r="C16" s="16">
+        <f>IF(B15=0,0,B16*(C15/B15))</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="153">
         <f>(D12/25)+(D11/100)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="16"/>
+      <c r="E16" s="16">
+        <f>IF(D15=0,0,D16*(E15/D15))</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="153">
+        <f>(F12/25)+(F11/100)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="16">
+        <f>IF(F15=0,0,F16*(G15/F15))</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <f>SUM(B16,D16,F16)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="16">
+        <f>SUM(C16,E16,G16)</f>
+        <v>0</v>
+      </c>
       <c r="J16" s="17"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -6841,19 +6864,19 @@
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="25" t="e">
-        <f>C13+C15</f>
+        <f>SUM(C13,C15,C16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E17" s="25" t="e">
-        <f>E13+E15</f>
+        <f>SUM(E13,E15,E16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G17" s="25">
-        <f>G13+G15</f>
+        <f>SUM(G13,G15,G16)</f>
         <v>0</v>
       </c>
       <c r="I17" s="34" t="e">
-        <f>I13+I15</f>
+        <f>I13+I15+I16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7180,20 +7203,38 @@
       <c r="A31" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="160">
+      <c r="B31" s="153">
         <f>(B27/25)+(B25/100)</f>
         <v>0</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="160">
+      <c r="C31" s="16">
+        <f>IF(B30=0,0,B31*(C30/B30))</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="153">
         <f>(D27/25)+(D25/100)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="16"/>
+      <c r="E31" s="16">
+        <f>IF(D30=0,0,D31*(E30/D30))</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="153">
+        <f>(F27/25)+(F25/100)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="16">
+        <f>IF(F30=0,0,F31*(G30/F30))</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="8">
+        <f>SUM(B31,D31,F31)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="16">
+        <f>SUM(C31,E31,G31)</f>
+        <v>0</v>
+      </c>
       <c r="J31" s="17"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
@@ -7205,19 +7246,19 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="25" t="e">
-        <f>C28+C30</f>
+        <f>C28+C30+C31</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E32" s="25" t="e">
-        <f>E28+E30</f>
+        <f>E28+E30+E31</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G32" s="25" t="e">
-        <f>G28+G30</f>
+        <f>G28+G30+G31</f>
         <v>#REF!</v>
       </c>
       <c r="I32" s="34" t="e">
-        <f>I28+I30</f>
+        <f>I28+I30+I31</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7246,13 +7287,12 @@
       <c r="J34" s="37"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="37" t="s">
-        <v>111</v>
-      </c>
       <c r="B35" s="37"/>
       <c r="C35" s="54"/>
       <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
+      <c r="E35" s="37" t="s">
+        <v>111</v>
+      </c>
       <c r="F35" s="37"/>
       <c r="G35" s="37"/>
       <c r="H35" s="37"/>
@@ -7264,7 +7304,9 @@
       <c r="B36" s="37"/>
       <c r="C36" s="54"/>
       <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
+      <c r="E36" s="37" t="s">
+        <v>128</v>
+      </c>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
       <c r="H36" s="37"/>
@@ -7288,12 +7330,11 @@
       <c r="B38" s="37"/>
       <c r="C38" s="54"/>
       <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="119" t="str">
+      <c r="E38" s="119" t="str">
         <f>Dashboard!$O$112</f>
         <v>Please see Key for Descriptions</v>
       </c>
+      <c r="F38" s="37"/>
       <c r="H38" s="37"/>
       <c r="I38" s="37"/>
       <c r="J38" s="37"/>
@@ -7750,7 +7791,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G38" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
+    <hyperlink ref="E38" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="74" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -7788,11 +7829,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="158" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
       <c r="F1" s="37"/>
@@ -8215,12 +8256,12 @@
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
       <c r="E28" s="37"/>
-      <c r="F28" s="155" t="s">
+      <c r="F28" s="157" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="155"/>
-      <c r="H28" s="155"/>
-      <c r="I28" s="155"/>
+      <c r="G28" s="157"/>
+      <c r="H28" s="157"/>
+      <c r="I28" s="157"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
@@ -8228,10 +8269,10 @@
       <c r="C29" s="37"/>
       <c r="D29" s="37"/>
       <c r="E29" s="37"/>
-      <c r="F29" s="155"/>
-      <c r="G29" s="155"/>
-      <c r="H29" s="155"/>
-      <c r="I29" s="155"/>
+      <c r="F29" s="157"/>
+      <c r="G29" s="157"/>
+      <c r="H29" s="157"/>
+      <c r="I29" s="157"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="37"/>
@@ -8452,11 +8493,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
       <c r="F1" s="37"/>
@@ -9998,11 +10039,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="160" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
       <c r="D1" s="44"/>
       <c r="E1" s="54"/>
       <c r="F1" s="70"/>
@@ -50102,10 +50143,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="161" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="159"/>
+      <c r="B1" s="161"/>
       <c r="C1" s="40"/>
       <c r="D1" s="37"/>
     </row>

</xml_diff>

<commit_message>
TICKET2383 - Updated template
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3718 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-9.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-9.xlsx
@@ -870,7 +870,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1188,6 +1188,7 @@
     <xf numFmtId="17" fontId="8" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1844,11 +1845,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="154645632"/>
-        <c:axId val="154647168"/>
+        <c:axId val="84672896"/>
+        <c:axId val="84674432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154645632"/>
+        <c:axId val="84672896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1876,7 +1877,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154647168"/>
+        <c:crossAx val="84674432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1884,7 +1885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154647168"/>
+        <c:axId val="84674432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +1913,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="154645632"/>
+        <c:crossAx val="84672896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2211,12 +2212,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="73007488"/>
-        <c:axId val="73009024"/>
+        <c:axId val="84716928"/>
+        <c:axId val="84718720"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="73007488"/>
+        <c:axId val="84716928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2244,7 +2245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73009024"/>
+        <c:crossAx val="84718720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2252,7 +2253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73009024"/>
+        <c:axId val="84718720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2280,7 +2281,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73007488"/>
+        <c:crossAx val="84716928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2498,12 +2499,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="73025408"/>
-        <c:axId val="73026944"/>
+        <c:axId val="85152896"/>
+        <c:axId val="85154432"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="73025408"/>
+        <c:axId val="85152896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2531,7 +2532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73026944"/>
+        <c:crossAx val="85154432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2539,7 +2540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73026944"/>
+        <c:axId val="85154432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2567,7 +2568,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73025408"/>
+        <c:crossAx val="85152896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2742,12 +2743,12 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="73043968"/>
-        <c:axId val="73045504"/>
+        <c:axId val="85185280"/>
+        <c:axId val="85186816"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="73043968"/>
+        <c:axId val="85185280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +2768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73045504"/>
+        <c:crossAx val="85186816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2775,7 +2776,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73045504"/>
+        <c:axId val="85186816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2785,7 +2786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73043968"/>
+        <c:crossAx val="85185280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4386,9 +4387,7 @@
   </sheetPr>
   <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6480,7 +6479,7 @@
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6497,10 +6496,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="156"/>
+      <c r="B1" s="157"/>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -6637,30 +6636,30 @@
       <c r="B10" s="8">
         <v>0</v>
       </c>
-      <c r="C10" s="16" t="e">
-        <f>C24/5</f>
-        <v>#DIV/0!</v>
+      <c r="C10" s="16">
+        <f>((Impressions!B34/1000)*Impressions!Q18)+((Impressions!C34/1000)*Impressions!Q19)+((Impressions!D34/1000)*Impressions!Q20)+((Impressions!E34/1000)*Impressions!Q21)</f>
+        <v>0</v>
       </c>
       <c r="D10" s="8">
         <v>0</v>
       </c>
-      <c r="E10" s="16" t="e">
-        <f>E24/5</f>
-        <v>#DIV/0!</v>
+      <c r="E10" s="16">
+        <f>((Impressions!B35/1000)*Impressions!Q18)+((Impressions!C35/1000)*Impressions!Q19)+((Impressions!D35/1000)*Impressions!Q20)+((Impressions!E35/1000)*Impressions!Q21)</f>
+        <v>0</v>
       </c>
       <c r="F10" s="8">
         <v>0</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="155">
         <v>0</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" ref="H10:I11" si="0">B10+D10+F10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="16" t="e">
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="J10" s="17">
         <v>0.1</v>
@@ -6747,14 +6746,14 @@
         <v>82</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="20" t="e">
+      <c r="C13" s="20">
         <f>SUM(C10:C12)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="20" t="e">
+      <c r="E13" s="20">
         <f>SUM(E10:E12)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="20">
@@ -6762,9 +6761,9 @@
         <v>0</v>
       </c>
       <c r="H13" s="8"/>
-      <c r="I13" s="20" t="e">
+      <c r="I13" s="20">
         <f>SUM(I10:I12)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="J13" s="17"/>
     </row>
@@ -6863,21 +6862,21 @@
         <v>71</v>
       </c>
       <c r="B17" s="8"/>
-      <c r="C17" s="25" t="e">
+      <c r="C17" s="25">
         <f>SUM(C13,C15,C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="E17" s="25">
         <f>SUM(E13,E15,E16)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="G17" s="25">
         <f>SUM(G13,G15,G16)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="34" t="e">
+      <c r="I17" s="34">
         <f>I13+I15+I16</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -6987,7 +6986,7 @@
       <c r="F24" s="8">
         <v>0</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="155">
         <v>0</v>
       </c>
       <c r="H24" s="8">
@@ -7829,11 +7828,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
       <c r="F1" s="37"/>
@@ -8256,12 +8255,12 @@
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
       <c r="E28" s="37"/>
-      <c r="F28" s="157" t="s">
+      <c r="F28" s="158" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
+      <c r="G28" s="158"/>
+      <c r="H28" s="158"/>
+      <c r="I28" s="158"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
@@ -8269,10 +8268,10 @@
       <c r="C29" s="37"/>
       <c r="D29" s="37"/>
       <c r="E29" s="37"/>
-      <c r="F29" s="157"/>
-      <c r="G29" s="157"/>
-      <c r="H29" s="157"/>
-      <c r="I29" s="157"/>
+      <c r="F29" s="158"/>
+      <c r="G29" s="158"/>
+      <c r="H29" s="158"/>
+      <c r="I29" s="158"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="37"/>
@@ -8493,11 +8492,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
       <c r="F1" s="37"/>
@@ -9474,7 +9473,7 @@
       <c r="P33" s="37"/>
       <c r="Q33" s="37"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="37"/>
       <c r="B34" s="37"/>
       <c r="C34" s="37"/>
@@ -9493,7 +9492,7 @@
       <c r="P34" s="37"/>
       <c r="Q34" s="37"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="37"/>
       <c r="B35" s="37"/>
       <c r="C35" s="37"/>
@@ -9512,7 +9511,7 @@
       <c r="P35" s="37"/>
       <c r="Q35" s="37"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="37"/>
       <c r="B36" s="37"/>
       <c r="C36" s="37"/>
@@ -10039,11 +10038,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
       <c r="D1" s="44"/>
       <c r="E1" s="54"/>
       <c r="F1" s="70"/>
@@ -50143,10 +50142,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="162" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="161"/>
+      <c r="B1" s="162"/>
       <c r="C1" s="40"/>
       <c r="D1" s="37"/>
     </row>

</xml_diff>

<commit_message>
TICKET2383 - Updated spreadsheet
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3730 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-9.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-9.xlsx
@@ -4250,9 +4250,7 @@
   </sheetPr>
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R80" sqref="R80"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>